<commit_message>
Fix nuts file errors
</commit_message>
<xml_diff>
--- a/data/nutrients.xlsx
+++ b/data/nutrients.xlsx
@@ -35144,11 +35144,11 @@
     <row r="1691">
       <c r="A1691" t="inlineStr">
         <is>
-          <t>72-3-1</t>
+          <t>72-1-25</t>
         </is>
       </c>
       <c r="B1691" t="n">
-        <v>0.02048724463456083</v>
+        <v>23.96503066558457</v>
       </c>
       <c r="C1691" t="inlineStr">
         <is>
@@ -35156,20 +35156,20 @@
         </is>
       </c>
       <c r="D1691" t="n">
-        <v>0.5019374935467404</v>
+        <v>30.20698997643281</v>
       </c>
       <c r="E1691" t="n">
-        <v>0.2048724463456083</v>
+        <v>1.586071628166357</v>
       </c>
     </row>
     <row r="1692">
       <c r="A1692" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>26</t>
         </is>
       </c>
       <c r="B1692" t="n">
-        <v>0.07170175601933437</v>
+        <v>23.40231747320941</v>
       </c>
       <c r="C1692" t="inlineStr">
         <is>
@@ -35177,134 +35177,146 @@
         </is>
       </c>
       <c r="D1692" t="n">
-        <v>0.5838571561574368</v>
+        <v>33.7578685369995</v>
       </c>
       <c r="E1692" t="n">
-        <v>0.2253483760607651</v>
+        <v>1.555379211162147</v>
       </c>
     </row>
     <row r="1693">
       <c r="A1693" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>27</t>
         </is>
       </c>
       <c r="B1693" t="n">
-        <v>11.26350079748654</v>
-      </c>
-      <c r="C1693" t="n">
-        <v>0.3174259315655299</v>
+        <v>23.47391210610701</v>
+      </c>
+      <c r="C1693" t="inlineStr">
+        <is>
+          <t>&lt;0.01</t>
+        </is>
       </c>
       <c r="D1693" t="n">
-        <v>1.955753320290845</v>
+        <v>38.15789810099086</v>
       </c>
       <c r="E1693" t="n">
-        <v>0.9010800637989237</v>
+        <v>1.565609656597372</v>
       </c>
     </row>
     <row r="1694">
       <c r="A1694" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>28</t>
         </is>
       </c>
       <c r="B1694" t="n">
-        <v>11.86536445834095</v>
-      </c>
-      <c r="C1694" t="n">
-        <v>0.05118793985479271</v>
+        <v>23.87288329059255</v>
+      </c>
+      <c r="C1694" t="inlineStr">
+        <is>
+          <t>&lt;0.01</t>
+        </is>
       </c>
       <c r="D1694" t="n">
-        <v>3.480779910125904</v>
+        <v>44.53269956307706</v>
       </c>
       <c r="E1694" t="n">
-        <v>0.8906701534733931</v>
+        <v>1.596300811544123</v>
       </c>
     </row>
     <row r="1695">
       <c r="A1695" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>29</t>
         </is>
       </c>
       <c r="B1695" t="n">
-        <v>17.89292519247975</v>
-      </c>
-      <c r="C1695" t="n">
-        <v>0.01023622722681908</v>
+        <v>24.04673259098046</v>
+      </c>
+      <c r="C1695" t="inlineStr">
+        <is>
+          <t>&lt;0.01</t>
+        </is>
       </c>
       <c r="D1695" t="n">
-        <v>5.179530976770454</v>
+        <v>49.11673039859839</v>
       </c>
       <c r="E1695" t="n">
-        <v>1.228347267218289</v>
+        <v>1.616759042287197</v>
       </c>
     </row>
     <row r="1696">
       <c r="A1696" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>30</t>
         </is>
       </c>
       <c r="B1696" t="n">
-        <v>26.90963039748042</v>
-      </c>
-      <c r="C1696" t="n">
-        <v>0.01023569052775976</v>
+        <v>24.06709124771226</v>
+      </c>
+      <c r="C1696" t="inlineStr">
+        <is>
+          <t>&lt;0.01</t>
+        </is>
       </c>
       <c r="D1696" t="n">
-        <v>8.096431207457972</v>
+        <v>51.0709406536275</v>
       </c>
       <c r="E1696" t="n">
-        <v>1.740067389719159</v>
+        <v>1.606519271212085</v>
       </c>
     </row>
     <row r="1697">
       <c r="A1697" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>31</t>
         </is>
       </c>
       <c r="B1697" t="n">
-        <v>29.8977454844801</v>
-      </c>
-      <c r="C1697" t="n">
-        <v>0.01023544864241017</v>
+        <v>23.98519496492469</v>
+      </c>
+      <c r="C1697" t="inlineStr">
+        <is>
+          <t>&lt;0.01</t>
+        </is>
       </c>
       <c r="D1697" t="n">
-        <v>9.355200059162893</v>
+        <v>51.65412294494019</v>
       </c>
       <c r="E1697" t="n">
-        <v>1.893557998845881</v>
+        <v>1.596284306539356</v>
       </c>
     </row>
     <row r="1698">
       <c r="A1698" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>32</t>
         </is>
       </c>
       <c r="B1698" t="n">
-        <v>30.50849261033586</v>
-      </c>
-      <c r="C1698" t="n">
-        <v>0.01023431486425222</v>
+        <v>23.92374640847356</v>
+      </c>
+      <c r="C1698" t="inlineStr">
+        <is>
+          <t>&lt;0.01</t>
+        </is>
       </c>
       <c r="D1698" t="n">
-        <v>12.43469256006644</v>
+        <v>52.27819520996212</v>
       </c>
       <c r="E1698" t="n">
-        <v>1.995691398529182</v>
+        <v>1.596280769769836</v>
       </c>
     </row>
     <row r="1699">
       <c r="A1699" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>33</t>
         </is>
       </c>
       <c r="B1699" t="n">
-        <v>32.93178764334375</v>
+        <v>23.94414081129887</v>
       </c>
       <c r="C1699" t="inlineStr">
         <is>
@@ -35312,20 +35324,20 @@
         </is>
       </c>
       <c r="D1699" t="n">
-        <v>12.58735202029609</v>
+        <v>52.74873755651525</v>
       </c>
       <c r="E1699" t="n">
-        <v>2.097892003382681</v>
+        <v>1.586043515278344</v>
       </c>
     </row>
     <row r="1700">
       <c r="A1700" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>34</t>
         </is>
       </c>
       <c r="B1700" t="n">
-        <v>33.0409654204282</v>
+        <v>23.91344319487413</v>
       </c>
       <c r="C1700" t="inlineStr">
         <is>
@@ -35333,20 +35345,20 @@
         </is>
       </c>
       <c r="D1700" t="n">
-        <v>14.04931728778195</v>
+        <v>53.26036449692762</v>
       </c>
       <c r="E1700" t="n">
-        <v>2.118141790656128</v>
+        <v>1.596276054086592</v>
       </c>
     </row>
     <row r="1701">
       <c r="A1701" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>72-3-1</t>
         </is>
       </c>
       <c r="B1701" t="n">
-        <v>38.39084107342094</v>
+        <v>0.02048724463456083</v>
       </c>
       <c r="C1701" t="inlineStr">
         <is>
@@ -35354,20 +35366,20 @@
         </is>
       </c>
       <c r="D1701" t="n">
-        <v>17.45596345182732</v>
+        <v>0.5019374935467404</v>
       </c>
       <c r="E1701" t="n">
-        <v>2.445472019335716</v>
+        <v>0.2048724463456083</v>
       </c>
     </row>
     <row r="1702">
       <c r="A1702" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B1702" t="n">
-        <v>38.3990028538813</v>
+        <v>0.07170175601933437</v>
       </c>
       <c r="C1702" t="inlineStr">
         <is>
@@ -35375,146 +35387,134 @@
         </is>
       </c>
       <c r="D1702" t="n">
-        <v>18.43725103722198</v>
+        <v>0.5838571561574368</v>
       </c>
       <c r="E1702" t="n">
-        <v>2.445340176412905</v>
+        <v>0.2253483760607651</v>
       </c>
     </row>
     <row r="1703">
       <c r="A1703" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="B1703" t="n">
-        <v>39.48182656502929</v>
-      </c>
-      <c r="C1703" t="inlineStr">
-        <is>
-          <t>&lt;0.01</t>
-        </is>
+        <v>11.26350079748654</v>
+      </c>
+      <c r="C1703" t="n">
+        <v>0.3174259315655299</v>
       </c>
       <c r="D1703" t="n">
-        <v>20.237121779121</v>
+        <v>1.955753320290845</v>
       </c>
       <c r="E1703" t="n">
-        <v>2.527082446634422</v>
+        <v>0.9010800637989237</v>
       </c>
     </row>
     <row r="1704">
       <c r="A1704" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="B1704" t="n">
-        <v>38.57912446868031</v>
-      </c>
-      <c r="C1704" t="inlineStr">
-        <is>
-          <t>&lt;0.01</t>
-        </is>
+        <v>11.86536445834095</v>
+      </c>
+      <c r="C1704" t="n">
+        <v>0.05118793985479271</v>
       </c>
       <c r="D1704" t="n">
-        <v>22.1285192855358</v>
+        <v>3.480779910125904</v>
       </c>
       <c r="E1704" t="n">
-        <v>2.496236109880137</v>
+        <v>0.8906701534733931</v>
       </c>
     </row>
     <row r="1705">
       <c r="A1705" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>5</t>
         </is>
       </c>
       <c r="B1705" t="n">
-        <v>37.46259144718095</v>
-      </c>
-      <c r="C1705" t="inlineStr">
-        <is>
-          <t>&lt;0.01</t>
-        </is>
+        <v>17.89292519247975</v>
+      </c>
+      <c r="C1705" t="n">
+        <v>0.01023622722681908</v>
       </c>
       <c r="D1705" t="n">
-        <v>23.73380998292185</v>
+        <v>5.179530976770454</v>
       </c>
       <c r="E1705" t="n">
-        <v>2.444991631861346</v>
+        <v>1.228347267218289</v>
       </c>
     </row>
     <row r="1706">
       <c r="A1706" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>6</t>
         </is>
       </c>
       <c r="B1706" t="n">
-        <v>37.44083153858018</v>
-      </c>
-      <c r="C1706" t="inlineStr">
-        <is>
-          <t>&lt;0.01</t>
-        </is>
+        <v>26.90963039748042</v>
+      </c>
+      <c r="C1706" t="n">
+        <v>0.01023569052775976</v>
       </c>
       <c r="D1706" t="n">
-        <v>26.34156863711584</v>
+        <v>8.096431207457972</v>
       </c>
       <c r="E1706" t="n">
-        <v>2.455136494333127</v>
+        <v>1.740067389719159</v>
       </c>
     </row>
     <row r="1707">
       <c r="A1707" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>7</t>
         </is>
       </c>
       <c r="B1707" t="n">
-        <v>37.70621981536882</v>
-      </c>
-      <c r="C1707" t="inlineStr">
-        <is>
-          <t>&lt;0.01</t>
-        </is>
+        <v>29.8977454844801</v>
+      </c>
+      <c r="C1707" t="n">
+        <v>0.01023544864241017</v>
       </c>
       <c r="D1707" t="n">
-        <v>28.8474063698698</v>
+        <v>9.355200059162893</v>
       </c>
       <c r="E1707" t="n">
-        <v>2.496016721364621</v>
+        <v>1.893557998845881</v>
       </c>
     </row>
     <row r="1708">
       <c r="A1708" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>8</t>
         </is>
       </c>
       <c r="B1708" t="n">
-        <v>36.6725720990914</v>
-      </c>
-      <c r="C1708" t="inlineStr">
-        <is>
-          <t>&lt;0.01</t>
-        </is>
+        <v>30.50849261033586</v>
+      </c>
+      <c r="C1708" t="n">
+        <v>0.01023431486425222</v>
       </c>
       <c r="D1708" t="n">
-        <v>30.50421478367937</v>
+        <v>12.43469256006644</v>
       </c>
       <c r="E1708" t="n">
-        <v>2.434608691655161</v>
+        <v>1.995691398529182</v>
       </c>
     </row>
     <row r="1709">
       <c r="A1709" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>9</t>
         </is>
       </c>
       <c r="B1709" t="n">
-        <v>36.40652577462653</v>
+        <v>32.93178764334375</v>
       </c>
       <c r="C1709" t="inlineStr">
         <is>
@@ -35522,20 +35522,20 @@
         </is>
       </c>
       <c r="D1709" t="n">
-        <v>32.87737393640058</v>
+        <v>12.58735202029609</v>
       </c>
       <c r="E1709" t="n">
-        <v>2.434603297095002</v>
+        <v>2.097892003382681</v>
       </c>
     </row>
     <row r="1710">
       <c r="A1710" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>10</t>
         </is>
       </c>
       <c r="B1710" t="n">
-        <v>35.77275054944941</v>
+        <v>33.0409654204282</v>
       </c>
       <c r="C1710" t="inlineStr">
         <is>
@@ -35543,20 +35543,20 @@
         </is>
       </c>
       <c r="D1710" t="n">
-        <v>36.10009627938432</v>
+        <v>14.04931728778195</v>
       </c>
       <c r="E1710" t="n">
-        <v>2.403945204209497</v>
+        <v>2.118141790656128</v>
       </c>
     </row>
     <row r="1711">
       <c r="A1711" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>11</t>
         </is>
       </c>
       <c r="B1711" t="n">
-        <v>34.62808909321948</v>
+        <v>38.39084107342094</v>
       </c>
       <c r="C1711" t="inlineStr">
         <is>
@@ -35564,20 +35564,20 @@
         </is>
       </c>
       <c r="D1711" t="n">
-        <v>38.93486176921517</v>
+        <v>17.45596345182732</v>
       </c>
       <c r="E1711" t="n">
-        <v>2.342638819009531</v>
+        <v>2.445472019335716</v>
       </c>
     </row>
     <row r="1712">
       <c r="A1712" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>12</t>
         </is>
       </c>
       <c r="B1712" t="n">
-        <v>33.4736225527866</v>
+        <v>38.3990028538813</v>
       </c>
       <c r="C1712" t="inlineStr">
         <is>
@@ -35585,20 +35585,20 @@
         </is>
       </c>
       <c r="D1712" t="n">
-        <v>39.31513797993854</v>
+        <v>18.43725103722198</v>
       </c>
       <c r="E1712" t="n">
-        <v>2.260901767776845</v>
+        <v>2.445340176412905</v>
       </c>
     </row>
     <row r="1713">
       <c r="A1713" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B1713" t="n">
-        <v>30.89834189447641</v>
+        <v>39.48182656502929</v>
       </c>
       <c r="C1713" t="inlineStr">
         <is>
@@ -35606,20 +35606,20 @@
         </is>
       </c>
       <c r="D1713" t="n">
-        <v>38.14205913331392</v>
+        <v>20.237121779121</v>
       </c>
       <c r="E1713" t="n">
-        <v>2.097404002770749</v>
+        <v>2.527082446634422</v>
       </c>
     </row>
     <row r="1714">
       <c r="A1714" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B1714" t="n">
-        <v>27.73893763924535</v>
+        <v>38.57912446868031</v>
       </c>
       <c r="C1714" t="inlineStr">
         <is>
@@ -35627,20 +35627,20 @@
         </is>
       </c>
       <c r="D1714" t="n">
-        <v>33.55071063042622</v>
+        <v>22.1285192855358</v>
       </c>
       <c r="E1714" t="n">
-        <v>1.862223035906549</v>
+        <v>2.496236109880137</v>
       </c>
     </row>
     <row r="1715">
       <c r="A1715" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>15</t>
         </is>
       </c>
       <c r="B1715" t="n">
-        <v>23.96503066558457</v>
+        <v>37.46259144718095</v>
       </c>
       <c r="C1715" t="inlineStr">
         <is>
@@ -35648,20 +35648,20 @@
         </is>
       </c>
       <c r="D1715" t="n">
-        <v>30.20698997643281</v>
+        <v>23.73380998292185</v>
       </c>
       <c r="E1715" t="n">
-        <v>1.586071628166357</v>
+        <v>2.444991631861346</v>
       </c>
     </row>
     <row r="1716">
       <c r="A1716" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>16</t>
         </is>
       </c>
       <c r="B1716" t="n">
-        <v>23.40231747320941</v>
+        <v>37.44083153858018</v>
       </c>
       <c r="C1716" t="inlineStr">
         <is>
@@ -35669,20 +35669,20 @@
         </is>
       </c>
       <c r="D1716" t="n">
-        <v>33.7578685369995</v>
+        <v>26.34156863711584</v>
       </c>
       <c r="E1716" t="n">
-        <v>1.555379211162147</v>
+        <v>2.455136494333127</v>
       </c>
     </row>
     <row r="1717">
       <c r="A1717" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>17</t>
         </is>
       </c>
       <c r="B1717" t="n">
-        <v>23.47391210610701</v>
+        <v>37.70621981536882</v>
       </c>
       <c r="C1717" t="inlineStr">
         <is>
@@ -35690,20 +35690,20 @@
         </is>
       </c>
       <c r="D1717" t="n">
-        <v>38.15789810099086</v>
+        <v>28.8474063698698</v>
       </c>
       <c r="E1717" t="n">
-        <v>1.565609656597372</v>
+        <v>2.496016721364621</v>
       </c>
     </row>
     <row r="1718">
       <c r="A1718" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>18</t>
         </is>
       </c>
       <c r="B1718" t="n">
-        <v>23.87288329059255</v>
+        <v>36.6725720990914</v>
       </c>
       <c r="C1718" t="inlineStr">
         <is>
@@ -35711,20 +35711,20 @@
         </is>
       </c>
       <c r="D1718" t="n">
-        <v>44.53269956307706</v>
+        <v>30.50421478367937</v>
       </c>
       <c r="E1718" t="n">
-        <v>1.596300811544123</v>
+        <v>2.434608691655161</v>
       </c>
     </row>
     <row r="1719">
       <c r="A1719" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>19</t>
         </is>
       </c>
       <c r="B1719" t="n">
-        <v>24.04673259098046</v>
+        <v>36.40652577462653</v>
       </c>
       <c r="C1719" t="inlineStr">
         <is>
@@ -35732,20 +35732,20 @@
         </is>
       </c>
       <c r="D1719" t="n">
-        <v>49.11673039859839</v>
+        <v>32.87737393640058</v>
       </c>
       <c r="E1719" t="n">
-        <v>1.616759042287197</v>
+        <v>2.434603297095002</v>
       </c>
     </row>
     <row r="1720">
       <c r="A1720" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>20</t>
         </is>
       </c>
       <c r="B1720" t="n">
-        <v>24.06709124771226</v>
+        <v>35.77275054944941</v>
       </c>
       <c r="C1720" t="inlineStr">
         <is>
@@ -35753,20 +35753,20 @@
         </is>
       </c>
       <c r="D1720" t="n">
-        <v>51.0709406536275</v>
+        <v>36.10009627938432</v>
       </c>
       <c r="E1720" t="n">
-        <v>1.606519271212085</v>
+        <v>2.403945204209497</v>
       </c>
     </row>
     <row r="1721">
       <c r="A1721" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>21</t>
         </is>
       </c>
       <c r="B1721" t="n">
-        <v>23.98519496492469</v>
+        <v>34.62808909321948</v>
       </c>
       <c r="C1721" t="inlineStr">
         <is>
@@ -35774,20 +35774,20 @@
         </is>
       </c>
       <c r="D1721" t="n">
-        <v>51.65412294494019</v>
+        <v>38.93486176921517</v>
       </c>
       <c r="E1721" t="n">
-        <v>1.596284306539356</v>
+        <v>2.342638819009531</v>
       </c>
     </row>
     <row r="1722">
       <c r="A1722" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>22</t>
         </is>
       </c>
       <c r="B1722" t="n">
-        <v>23.92374640847356</v>
+        <v>33.4736225527866</v>
       </c>
       <c r="C1722" t="inlineStr">
         <is>
@@ -35795,20 +35795,20 @@
         </is>
       </c>
       <c r="D1722" t="n">
-        <v>52.27819520996212</v>
+        <v>39.31513797993854</v>
       </c>
       <c r="E1722" t="n">
-        <v>1.596280769769836</v>
+        <v>2.260901767776845</v>
       </c>
     </row>
     <row r="1723">
       <c r="A1723" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>23</t>
         </is>
       </c>
       <c r="B1723" t="n">
-        <v>23.94414081129887</v>
+        <v>30.89834189447641</v>
       </c>
       <c r="C1723" t="inlineStr">
         <is>
@@ -35816,20 +35816,20 @@
         </is>
       </c>
       <c r="D1723" t="n">
-        <v>52.74873755651525</v>
+        <v>38.14205913331392</v>
       </c>
       <c r="E1723" t="n">
-        <v>1.586043515278344</v>
+        <v>2.097404002770749</v>
       </c>
     </row>
     <row r="1724">
       <c r="A1724" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>24</t>
         </is>
       </c>
       <c r="B1724" t="n">
-        <v>23.91344319487413</v>
+        <v>27.73893763924535</v>
       </c>
       <c r="C1724" t="inlineStr">
         <is>
@@ -35837,10 +35837,10 @@
         </is>
       </c>
       <c r="D1724" t="n">
-        <v>53.26036449692762</v>
+        <v>33.55071063042622</v>
       </c>
       <c r="E1724" t="n">
-        <v>1.596276054086592</v>
+        <v>1.862223035906549</v>
       </c>
     </row>
     <row r="1725">
@@ -40315,125 +40315,145 @@
     <row r="1940">
       <c r="A1940" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B1940" t="n">
-        <v>0.03074203243953507</v>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B1940" t="inlineStr">
+        <is>
+          <t>n.a.</t>
+        </is>
       </c>
       <c r="C1940" t="inlineStr">
         <is>
-          <t>&lt;0.01</t>
+          <t>n.a.</t>
         </is>
       </c>
       <c r="D1940" t="n">
-        <v>0.7173140902558183</v>
+        <v>10.50068622309955</v>
       </c>
       <c r="E1940" t="n">
-        <v>0.163957506344187</v>
+        <v>1.952963884105122</v>
       </c>
     </row>
     <row r="1941">
       <c r="A1941" t="inlineStr">
         <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B1941" t="n">
-        <v>0.1434530735778146</v>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="B1941" t="inlineStr">
+        <is>
+          <t>n.a.</t>
+        </is>
       </c>
       <c r="C1941" t="inlineStr">
         <is>
-          <t>&lt;0.01</t>
+          <t>n.a.</t>
         </is>
       </c>
       <c r="D1941" t="n">
-        <v>0.6557854792128666</v>
+        <v>14.28139601828034</v>
       </c>
       <c r="E1941" t="n">
-        <v>0.1844396660286187</v>
+        <v>2.254057825269856</v>
       </c>
     </row>
     <row r="1942">
       <c r="A1942" t="inlineStr">
         <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="B1942" t="n">
-        <v>9.96594801460976</v>
-      </c>
-      <c r="C1942" t="n">
-        <v>0.5018822741170382</v>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="B1942" t="inlineStr">
+        <is>
+          <t>n.a.</t>
+        </is>
+      </c>
+      <c r="C1942" t="inlineStr">
+        <is>
+          <t>n.a.</t>
+        </is>
       </c>
       <c r="D1942" t="n">
-        <v>2.335288948952749</v>
+        <v>17.77208285482256</v>
       </c>
       <c r="E1942" t="n">
-        <v>0.7989146404312037</v>
+        <v>2.444953191409897</v>
       </c>
     </row>
     <row r="1943">
       <c r="A1943" t="inlineStr">
         <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="B1943" t="n">
-        <v>29.55506526931747</v>
-      </c>
-      <c r="C1943" t="n">
-        <v>0.06142375878625036</v>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="B1943" t="inlineStr">
+        <is>
+          <t>n.a.</t>
+        </is>
+      </c>
+      <c r="C1943" t="inlineStr">
+        <is>
+          <t>n.a.</t>
+        </is>
       </c>
       <c r="D1943" t="n">
-        <v>7.002308501632541</v>
+        <v>21.20078207613208</v>
       </c>
       <c r="E1943" t="n">
-        <v>1.945085694897928</v>
+        <v>2.546815308470012</v>
       </c>
     </row>
     <row r="1944">
       <c r="A1944" t="inlineStr">
         <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="B1944" t="n">
-        <v>31.64097280260479</v>
-      </c>
-      <c r="C1944" t="n">
-        <v>0.02047296849084749</v>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B1944" t="inlineStr">
+        <is>
+          <t>n.a.</t>
+        </is>
+      </c>
+      <c r="C1944" t="inlineStr">
+        <is>
+          <t>n.a.</t>
+        </is>
       </c>
       <c r="D1944" t="n">
-        <v>9.069525041445438</v>
+        <v>28.03772089030626</v>
       </c>
       <c r="E1944" t="n">
-        <v>2.016587396348478</v>
+        <v>2.564293452850653</v>
       </c>
     </row>
     <row r="1945">
       <c r="A1945" t="inlineStr">
         <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="B1945" t="n">
-        <v>30.29844945617392</v>
-      </c>
-      <c r="C1945" t="n">
-        <v>0.01023596265411281</v>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="B1945" t="inlineStr">
+        <is>
+          <t>n.a.</t>
+        </is>
+      </c>
+      <c r="C1945" t="inlineStr">
+        <is>
+          <t>n.a.</t>
+        </is>
       </c>
       <c r="D1945" t="n">
-        <v>8.935995397040482</v>
+        <v>34.48750693060529</v>
       </c>
       <c r="E1945" t="n">
-        <v>1.924360978973208</v>
+        <v>2.489099215838068</v>
       </c>
     </row>
     <row r="1946">
       <c r="A1946" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>28</t>
         </is>
       </c>
       <c r="B1946" t="inlineStr">
@@ -40447,60 +40467,66 @@
         </is>
       </c>
       <c r="D1946" t="n">
-        <v>10.50068622309955</v>
+        <v>35.95378449797155</v>
       </c>
       <c r="E1946" t="n">
-        <v>1.952963884105122</v>
+        <v>2.292702132998158</v>
       </c>
     </row>
     <row r="1947">
       <c r="A1947" t="inlineStr">
         <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="B1947" t="n">
-        <v>30.70430509131183</v>
-      </c>
-      <c r="C1947" t="n">
-        <v>0.01023476836377061</v>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="B1947" t="inlineStr">
+        <is>
+          <t>n.a.</t>
+        </is>
+      </c>
+      <c r="C1947" t="inlineStr">
+        <is>
+          <t>n.a.</t>
+        </is>
       </c>
       <c r="D1947" t="n">
-        <v>10.53157664631996</v>
+        <v>33.76446033921046</v>
       </c>
       <c r="E1947" t="n">
-        <v>1.954840757480186</v>
+        <v>2.053186138263443</v>
       </c>
     </row>
     <row r="1948">
       <c r="A1948" t="inlineStr">
         <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="B1948" t="n">
-        <v>35.1940933369585</v>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="B1948" t="inlineStr">
+        <is>
+          <t>n.a.</t>
+        </is>
       </c>
       <c r="C1948" t="inlineStr">
         <is>
-          <t>&lt;0.01</t>
+          <t>n.a.</t>
         </is>
       </c>
       <c r="D1948" t="n">
-        <v>13.3653637388973</v>
+        <v>29.63595495801888</v>
       </c>
       <c r="E1948" t="n">
-        <v>2.230971895160498</v>
+        <v>1.804065607377795</v>
       </c>
     </row>
     <row r="1949">
       <c r="A1949" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>37</t>
         </is>
       </c>
       <c r="B1949" t="n">
-        <v>35.65264021949117</v>
+        <v>24.95756765882103</v>
       </c>
       <c r="C1949" t="inlineStr">
         <is>
@@ -40508,43 +40534,41 @@
         </is>
       </c>
       <c r="D1949" t="n">
-        <v>14.23444963987147</v>
+        <v>28.42645467659075</v>
       </c>
       <c r="E1949" t="n">
-        <v>2.251314824422519</v>
+        <v>1.647465515813935</v>
       </c>
     </row>
     <row r="1950">
       <c r="A1950" t="inlineStr">
         <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="B1950" t="inlineStr">
-        <is>
-          <t>n.a.</t>
-        </is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="B1950" t="n">
+        <v>23.94475975021849</v>
       </c>
       <c r="C1950" t="inlineStr">
         <is>
-          <t>n.a.</t>
+          <t>&lt;0.01</t>
         </is>
       </c>
       <c r="D1950" t="n">
-        <v>14.28139601828034</v>
+        <v>29.70582801490781</v>
       </c>
       <c r="E1950" t="n">
-        <v>2.254057825269856</v>
+        <v>1.586084513369174</v>
       </c>
     </row>
     <row r="1951">
       <c r="A1951" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>39</t>
         </is>
       </c>
       <c r="B1951" t="n">
-        <v>37.20534623971833</v>
+        <v>23.68902714360828</v>
       </c>
       <c r="C1951" t="inlineStr">
         <is>
@@ -40552,43 +40576,41 @@
         </is>
       </c>
       <c r="D1951" t="n">
-        <v>15.99338728621555</v>
+        <v>33.12370663665659</v>
       </c>
       <c r="E1951" t="n">
-        <v>2.353473497011886</v>
+        <v>1.565624688108884</v>
       </c>
     </row>
     <row r="1952">
       <c r="A1952" t="inlineStr">
         <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="B1952" t="inlineStr">
-        <is>
-          <t>n.a.</t>
-        </is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="B1952" t="n">
+        <v>23.46374867882316</v>
       </c>
       <c r="C1952" t="inlineStr">
         <is>
-          <t>n.a.</t>
+          <t>&lt;0.01</t>
         </is>
       </c>
       <c r="D1952" t="n">
-        <v>17.77208285482256</v>
+        <v>37.66683771772702</v>
       </c>
       <c r="E1952" t="n">
-        <v>2.444953191409897</v>
+        <v>1.555381508583132</v>
       </c>
     </row>
     <row r="1953">
       <c r="A1953" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>41</t>
         </is>
       </c>
       <c r="B1953" t="n">
-        <v>38.51297206558605</v>
+        <v>23.67847952542513</v>
       </c>
       <c r="C1953" t="inlineStr">
         <is>
@@ -40596,20 +40618,20 @@
         </is>
       </c>
       <c r="D1953" t="n">
-        <v>17.78308858926369</v>
+        <v>42.17921028686359</v>
       </c>
       <c r="E1953" t="n">
-        <v>2.445430479191038</v>
+        <v>1.565603875276596</v>
       </c>
     </row>
     <row r="1954">
       <c r="A1954" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>42</t>
         </is>
       </c>
       <c r="B1954" t="n">
-        <v>39.25764111227714</v>
+        <v>24.40487541680358</v>
       </c>
       <c r="C1954" t="inlineStr">
         <is>
@@ -40617,43 +40639,41 @@
         </is>
       </c>
       <c r="D1954" t="n">
-        <v>19.55208552659933</v>
+        <v>48.92231000743728</v>
       </c>
       <c r="E1954" t="n">
-        <v>2.516908968887198</v>
+        <v>1.616759042287197</v>
       </c>
     </row>
     <row r="1955">
       <c r="A1955" t="inlineStr">
         <is>
-          <t>19</t>
-        </is>
-      </c>
-      <c r="B1955" t="inlineStr">
-        <is>
-          <t>n.a.</t>
-        </is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="B1955" t="n">
+        <v>24.18990039484966</v>
       </c>
       <c r="C1955" t="inlineStr">
         <is>
-          <t>n.a.</t>
+          <t>&lt;0.01</t>
         </is>
       </c>
       <c r="D1955" t="n">
-        <v>21.20078207613208</v>
+        <v>51.94075059401729</v>
       </c>
       <c r="E1955" t="n">
-        <v>2.546815308470012</v>
+        <v>1.6167530720754</v>
       </c>
     </row>
     <row r="1956">
       <c r="A1956" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>44</t>
         </is>
       </c>
       <c r="B1956" t="n">
-        <v>39.03964005102906</v>
+        <v>24.21036562361011</v>
       </c>
       <c r="C1956" t="inlineStr">
         <is>
@@ -40661,20 +40681,20 @@
         </is>
       </c>
       <c r="D1956" t="n">
-        <v>22.70150976761884</v>
+        <v>51.94075059401729</v>
       </c>
       <c r="E1956" t="n">
-        <v>2.557628410051694</v>
+        <v>1.6167530720754</v>
       </c>
     </row>
     <row r="1957">
       <c r="A1957" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>45</t>
         </is>
       </c>
       <c r="B1957" t="n">
-        <v>38.25994507967889</v>
+        <v>24.05676980595438</v>
       </c>
       <c r="C1957" t="inlineStr">
         <is>
@@ -40682,16 +40702,16 @@
         </is>
       </c>
       <c r="D1957" t="n">
-        <v>26.16816564540604</v>
+        <v>53.06610302581004</v>
       </c>
       <c r="E1957" t="n">
-        <v>2.56771289171107</v>
+        <v>1.596280769769836</v>
       </c>
     </row>
     <row r="1958">
       <c r="A1958" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>46</t>
         </is>
       </c>
       <c r="B1958" t="inlineStr">
@@ -40705,20 +40725,20 @@
         </is>
       </c>
       <c r="D1958" t="n">
-        <v>28.03772089030626</v>
+        <v>53.4353803748889</v>
       </c>
       <c r="E1958" t="n">
-        <v>2.564293452850653</v>
+        <v>1.589216776014246</v>
       </c>
     </row>
     <row r="1959">
       <c r="A1959" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>47</t>
         </is>
       </c>
       <c r="B1959" t="n">
-        <v>38.71917669196453</v>
+        <v>23.974803014817</v>
       </c>
       <c r="C1959" t="inlineStr">
         <is>
@@ -40726,20 +40746,20 @@
         </is>
       </c>
       <c r="D1959" t="n">
-        <v>29.94214799930784</v>
+        <v>53.67981929822022</v>
       </c>
       <c r="E1959" t="n">
-        <v>2.557409292732135</v>
+        <v>1.586041172555115</v>
       </c>
     </row>
     <row r="1960">
       <c r="A1960" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>48</t>
         </is>
       </c>
       <c r="B1960" t="n">
-        <v>38.41225920586627</v>
+        <v>23.974803014817</v>
       </c>
       <c r="C1960" t="inlineStr">
         <is>
@@ -40747,43 +40767,41 @@
         </is>
       </c>
       <c r="D1960" t="n">
-        <v>33.22583699085317</v>
+        <v>53.92539986687392</v>
       </c>
       <c r="E1960" t="n">
-        <v>2.526718515006384</v>
+        <v>1.586041172555115</v>
       </c>
     </row>
     <row r="1961">
       <c r="A1961" t="inlineStr">
         <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="B1961" t="inlineStr">
-        <is>
-          <t>n.a.</t>
-        </is>
+          <t>82-2-2</t>
+        </is>
+      </c>
+      <c r="B1961" t="n">
+        <v>0.03074203243953507</v>
       </c>
       <c r="C1961" t="inlineStr">
         <is>
-          <t>n.a.</t>
+          <t>&lt;0.01</t>
         </is>
       </c>
       <c r="D1961" t="n">
-        <v>34.48750693060529</v>
+        <v>0.7173140902558183</v>
       </c>
       <c r="E1961" t="n">
-        <v>2.489099215838068</v>
+        <v>0.163957506344187</v>
       </c>
     </row>
     <row r="1962">
       <c r="A1962" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>3</t>
         </is>
       </c>
       <c r="B1962" t="n">
-        <v>36.82753701883523</v>
+        <v>0.1434530735778146</v>
       </c>
       <c r="C1962" t="inlineStr">
         <is>
@@ -40791,131 +40809,115 @@
         </is>
       </c>
       <c r="D1962" t="n">
-        <v>35.42604463784067</v>
+        <v>0.6557854792128666</v>
       </c>
       <c r="E1962" t="n">
-        <v>2.444939263194895</v>
+        <v>0.1844396660286187</v>
       </c>
     </row>
     <row r="1963">
       <c r="A1963" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>5</t>
         </is>
       </c>
       <c r="B1963" t="n">
-        <v>35.41748888797317</v>
-      </c>
-      <c r="C1963" t="inlineStr">
-        <is>
-          <t>&lt;0.01</t>
-        </is>
+        <v>9.96594801460976</v>
+      </c>
+      <c r="C1963" t="n">
+        <v>0.5018822741170382</v>
       </c>
       <c r="D1963" t="n">
-        <v>36.13361373550585</v>
+        <v>2.335288948952749</v>
       </c>
       <c r="E1963" t="n">
-        <v>2.352981641893076</v>
+        <v>0.7989146404312037</v>
       </c>
     </row>
     <row r="1964">
       <c r="A1964" t="inlineStr">
         <is>
-          <t>28</t>
-        </is>
-      </c>
-      <c r="B1964" t="inlineStr">
-        <is>
-          <t>n.a.</t>
-        </is>
-      </c>
-      <c r="C1964" t="inlineStr">
-        <is>
-          <t>n.a.</t>
-        </is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B1964" t="n">
+        <v>29.55506526931747</v>
+      </c>
+      <c r="C1964" t="n">
+        <v>0.06142375878625036</v>
       </c>
       <c r="D1964" t="n">
-        <v>35.95378449797155</v>
+        <v>7.002308501632541</v>
       </c>
       <c r="E1964" t="n">
-        <v>2.292702132998158</v>
+        <v>1.945085694897928</v>
       </c>
     </row>
     <row r="1965">
       <c r="A1965" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>8</t>
         </is>
       </c>
       <c r="B1965" t="n">
-        <v>33.45489148596553</v>
-      </c>
-      <c r="C1965" t="inlineStr">
-        <is>
-          <t>&lt;0.01</t>
-        </is>
+        <v>31.64097280260479</v>
+      </c>
+      <c r="C1965" t="n">
+        <v>0.02047296849084749</v>
       </c>
       <c r="D1965" t="n">
-        <v>35.57267819471014</v>
+        <v>9.069525041445438</v>
       </c>
       <c r="E1965" t="n">
-        <v>2.230326099064369</v>
+        <v>2.016587396348478</v>
       </c>
     </row>
     <row r="1966">
       <c r="A1966" t="inlineStr">
         <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="B1966" t="inlineStr">
-        <is>
-          <t>n.a.</t>
-        </is>
-      </c>
-      <c r="C1966" t="inlineStr">
-        <is>
-          <t>n.a.</t>
-        </is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="B1966" t="n">
+        <v>30.29844945617392</v>
+      </c>
+      <c r="C1966" t="n">
+        <v>0.01023596265411281</v>
       </c>
       <c r="D1966" t="n">
-        <v>34.47574323308977</v>
+        <v>8.935995397040482</v>
       </c>
       <c r="E1966" t="n">
-        <v>2.112989818523772</v>
+        <v>1.924360978973208</v>
       </c>
     </row>
     <row r="1967">
       <c r="A1967" t="inlineStr">
         <is>
-          <t>31</t>
-        </is>
-      </c>
-      <c r="B1967" t="inlineStr">
-        <is>
-          <t>n.a.</t>
-        </is>
-      </c>
-      <c r="C1967" t="inlineStr">
-        <is>
-          <t>n.a.</t>
-        </is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="B1967" t="n">
+        <v>30.70430509131183</v>
+      </c>
+      <c r="C1967" t="n">
+        <v>0.01023476836377061</v>
       </c>
       <c r="D1967" t="n">
-        <v>33.76446033921046</v>
+        <v>10.53157664631996</v>
       </c>
       <c r="E1967" t="n">
-        <v>2.053186138263443</v>
+        <v>1.954840757480186</v>
       </c>
     </row>
     <row r="1968">
       <c r="A1968" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>12</t>
         </is>
       </c>
       <c r="B1968" t="n">
-        <v>29.92774456925275</v>
+        <v>35.1940933369585</v>
       </c>
       <c r="C1968" t="inlineStr">
         <is>
@@ -40923,20 +40925,20 @@
         </is>
       </c>
       <c r="D1968" t="n">
-        <v>32.95633000258568</v>
+        <v>13.3653637388973</v>
       </c>
       <c r="E1968" t="n">
-        <v>1.995182971283517</v>
+        <v>2.230971895160498</v>
       </c>
     </row>
     <row r="1969">
       <c r="A1969" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B1969" t="n">
-        <v>27.95428437427739</v>
+        <v>35.65264021949117</v>
       </c>
       <c r="C1969" t="inlineStr">
         <is>
@@ -40944,43 +40946,41 @@
         </is>
       </c>
       <c r="D1969" t="n">
-        <v>30.46116565967196</v>
+        <v>14.23444963987147</v>
       </c>
       <c r="E1969" t="n">
-        <v>1.862254669150251</v>
+        <v>2.251314824422519</v>
       </c>
     </row>
     <row r="1970">
       <c r="A1970" t="inlineStr">
         <is>
-          <t>34</t>
-        </is>
-      </c>
-      <c r="B1970" t="inlineStr">
-        <is>
-          <t>n.a.</t>
-        </is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="B1970" t="n">
+        <v>37.20534623971833</v>
       </c>
       <c r="C1970" t="inlineStr">
         <is>
-          <t>n.a.</t>
+          <t>&lt;0.01</t>
         </is>
       </c>
       <c r="D1970" t="n">
-        <v>29.63595495801888</v>
+        <v>15.99338728621555</v>
       </c>
       <c r="E1970" t="n">
-        <v>1.804065607377795</v>
+        <v>2.353473497011886</v>
       </c>
     </row>
     <row r="1971">
       <c r="A1971" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>17</t>
         </is>
       </c>
       <c r="B1971" t="n">
-        <v>26.3178565709324</v>
+        <v>38.51297206558605</v>
       </c>
       <c r="C1971" t="inlineStr">
         <is>
@@ -40988,20 +40988,20 @@
         </is>
       </c>
       <c r="D1971" t="n">
-        <v>28.97829308276849</v>
+        <v>17.78308858926369</v>
       </c>
       <c r="E1971" t="n">
-        <v>1.749748628938351</v>
+        <v>2.445430479191038</v>
       </c>
     </row>
     <row r="1972">
       <c r="A1972" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>18</t>
         </is>
       </c>
       <c r="B1972" t="n">
-        <v>24.90634895033802</v>
+        <v>39.25764111227714</v>
       </c>
       <c r="C1972" t="inlineStr">
         <is>
@@ -41009,20 +41009,20 @@
         </is>
       </c>
       <c r="D1972" t="n">
-        <v>28.40592632955561</v>
+        <v>19.55208552659933</v>
       </c>
       <c r="E1972" t="n">
-        <v>1.647461865655062</v>
+        <v>2.516908968887198</v>
       </c>
     </row>
     <row r="1973">
       <c r="A1973" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>20</t>
         </is>
       </c>
       <c r="B1973" t="n">
-        <v>24.95756765882103</v>
+        <v>39.03964005102906</v>
       </c>
       <c r="C1973" t="inlineStr">
         <is>
@@ -41030,20 +41030,20 @@
         </is>
       </c>
       <c r="D1973" t="n">
-        <v>28.42645467659075</v>
+        <v>22.70150976761884</v>
       </c>
       <c r="E1973" t="n">
-        <v>1.647465515813935</v>
+        <v>2.557628410051694</v>
       </c>
     </row>
     <row r="1974">
       <c r="A1974" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>21</t>
         </is>
       </c>
       <c r="B1974" t="n">
-        <v>23.94475975021849</v>
+        <v>38.25994507967889</v>
       </c>
       <c r="C1974" t="inlineStr">
         <is>
@@ -41051,20 +41051,20 @@
         </is>
       </c>
       <c r="D1974" t="n">
-        <v>29.70582801490781</v>
+        <v>26.16816564540604</v>
       </c>
       <c r="E1974" t="n">
-        <v>1.586084513369174</v>
+        <v>2.56771289171107</v>
       </c>
     </row>
     <row r="1975">
       <c r="A1975" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>23</t>
         </is>
       </c>
       <c r="B1975" t="n">
-        <v>23.68902714360828</v>
+        <v>38.71917669196453</v>
       </c>
       <c r="C1975" t="inlineStr">
         <is>
@@ -41072,20 +41072,20 @@
         </is>
       </c>
       <c r="D1975" t="n">
-        <v>33.12370663665659</v>
+        <v>29.94214799930784</v>
       </c>
       <c r="E1975" t="n">
-        <v>1.565624688108884</v>
+        <v>2.557409292732135</v>
       </c>
     </row>
     <row r="1976">
       <c r="A1976" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>24</t>
         </is>
       </c>
       <c r="B1976" t="n">
-        <v>23.46374867882316</v>
+        <v>38.41225920586627</v>
       </c>
       <c r="C1976" t="inlineStr">
         <is>
@@ -41093,20 +41093,20 @@
         </is>
       </c>
       <c r="D1976" t="n">
-        <v>37.66683771772702</v>
+        <v>33.22583699085317</v>
       </c>
       <c r="E1976" t="n">
-        <v>1.555381508583132</v>
+        <v>2.526718515006384</v>
       </c>
     </row>
     <row r="1977">
       <c r="A1977" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>26</t>
         </is>
       </c>
       <c r="B1977" t="n">
-        <v>23.67847952542513</v>
+        <v>36.82753701883523</v>
       </c>
       <c r="C1977" t="inlineStr">
         <is>
@@ -41114,20 +41114,20 @@
         </is>
       </c>
       <c r="D1977" t="n">
-        <v>42.17921028686359</v>
+        <v>35.42604463784067</v>
       </c>
       <c r="E1977" t="n">
-        <v>1.565603875276596</v>
+        <v>2.444939263194895</v>
       </c>
     </row>
     <row r="1978">
       <c r="A1978" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>27</t>
         </is>
       </c>
       <c r="B1978" t="n">
-        <v>24.40487541680358</v>
+        <v>35.41748888797317</v>
       </c>
       <c r="C1978" t="inlineStr">
         <is>
@@ -41135,20 +41135,20 @@
         </is>
       </c>
       <c r="D1978" t="n">
-        <v>48.92231000743728</v>
+        <v>36.13361373550585</v>
       </c>
       <c r="E1978" t="n">
-        <v>1.616759042287197</v>
+        <v>2.352981641893076</v>
       </c>
     </row>
     <row r="1979">
       <c r="A1979" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>29</t>
         </is>
       </c>
       <c r="B1979" t="n">
-        <v>24.18990039484966</v>
+        <v>33.45489148596553</v>
       </c>
       <c r="C1979" t="inlineStr">
         <is>
@@ -41156,41 +41156,43 @@
         </is>
       </c>
       <c r="D1979" t="n">
-        <v>51.94075059401729</v>
+        <v>35.57267819471014</v>
       </c>
       <c r="E1979" t="n">
-        <v>1.6167530720754</v>
+        <v>2.230326099064369</v>
       </c>
     </row>
     <row r="1980">
       <c r="A1980" t="inlineStr">
         <is>
-          <t>44</t>
-        </is>
-      </c>
-      <c r="B1980" t="n">
-        <v>24.21036562361011</v>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="B1980" t="inlineStr">
+        <is>
+          <t>n.a.</t>
+        </is>
       </c>
       <c r="C1980" t="inlineStr">
         <is>
-          <t>&lt;0.01</t>
+          <t>n.a.</t>
         </is>
       </c>
       <c r="D1980" t="n">
-        <v>51.94075059401729</v>
+        <v>34.47574323308977</v>
       </c>
       <c r="E1980" t="n">
-        <v>1.6167530720754</v>
+        <v>2.112989818523772</v>
       </c>
     </row>
     <row r="1981">
       <c r="A1981" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>32</t>
         </is>
       </c>
       <c r="B1981" t="n">
-        <v>24.05676980595438</v>
+        <v>29.92774456925275</v>
       </c>
       <c r="C1981" t="inlineStr">
         <is>
@@ -41198,43 +41200,41 @@
         </is>
       </c>
       <c r="D1981" t="n">
-        <v>53.06610302581004</v>
+        <v>32.95633000258568</v>
       </c>
       <c r="E1981" t="n">
-        <v>1.596280769769836</v>
+        <v>1.995182971283517</v>
       </c>
     </row>
     <row r="1982">
       <c r="A1982" t="inlineStr">
         <is>
-          <t>46</t>
-        </is>
-      </c>
-      <c r="B1982" t="inlineStr">
-        <is>
-          <t>n.a.</t>
-        </is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="B1982" t="n">
+        <v>27.95428437427739</v>
       </c>
       <c r="C1982" t="inlineStr">
         <is>
-          <t>n.a.</t>
+          <t>&lt;0.01</t>
         </is>
       </c>
       <c r="D1982" t="n">
-        <v>53.4353803748889</v>
+        <v>30.46116565967196</v>
       </c>
       <c r="E1982" t="n">
-        <v>1.589216776014246</v>
+        <v>1.862254669150251</v>
       </c>
     </row>
     <row r="1983">
       <c r="A1983" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>35</t>
         </is>
       </c>
       <c r="B1983" t="n">
-        <v>23.974803014817</v>
+        <v>26.3178565709324</v>
       </c>
       <c r="C1983" t="inlineStr">
         <is>
@@ -41242,20 +41242,20 @@
         </is>
       </c>
       <c r="D1983" t="n">
-        <v>53.67981929822022</v>
+        <v>28.97829308276849</v>
       </c>
       <c r="E1983" t="n">
-        <v>1.586041172555115</v>
+        <v>1.749748628938351</v>
       </c>
     </row>
     <row r="1984">
       <c r="A1984" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>36</t>
         </is>
       </c>
       <c r="B1984" t="n">
-        <v>23.974803014817</v>
+        <v>24.90634895033802</v>
       </c>
       <c r="C1984" t="inlineStr">
         <is>
@@ -41263,10 +41263,10 @@
         </is>
       </c>
       <c r="D1984" t="n">
-        <v>53.92539986687392</v>
+        <v>28.40592632955561</v>
       </c>
       <c r="E1984" t="n">
-        <v>1.586041172555115</v>
+        <v>1.647461865655062</v>
       </c>
     </row>
     <row r="1985">

</xml_diff>